<commit_message>
minor update: two date entries fixed
</commit_message>
<xml_diff>
--- a/answers.xlsx
+++ b/answers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ja_nnik/uvprojects/KVG_Ulf_Selfassessment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BD2E37-1F24-FB43-9745-EA28A951BD9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151F4BE5-F58B-5D48-8AED-2E8EE15DA403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1191,22 +1191,6 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF5B3F86"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF5B3F86"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF5B3F86"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF5B3F86"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF8F9FA"/>
@@ -1230,13 +1214,29 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF5B3F86"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B3F86"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B3F86"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B3F86"/>
+        </bottom>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Formularantworten 1-style" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" size="0" dxfId="0"/>
-      <tableStyleElement type="headerRow" dxfId="3"/>
-      <tableStyleElement type="firstRowStripe" dxfId="2"/>
-      <tableStyleElement type="secondRowStripe" dxfId="1"/>
+      <tableStyleElement type="wholeTable" size="0" dxfId="3"/>
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1480,8 +1480,8 @@
   <dimension ref="A1:R52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2127,7 +2127,7 @@
         <v>45965</v>
       </c>
       <c r="F12" s="4">
-        <v>45684</v>
+        <v>46049</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>93</v>
@@ -4196,10 +4196,10 @@
         <v>65</v>
       </c>
       <c r="E49" s="4">
-        <v>46070</v>
+        <v>45978</v>
       </c>
       <c r="F49" s="4">
-        <v>46049</v>
+        <v>46048</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>248</v>

</xml_diff>